<commit_message>
Include subtotal lines to break down key sections in the income statements.
</commit_message>
<xml_diff>
--- a/public/uploads/media/default/sample_project_tasks.xlsx
+++ b/public/uploads/media/default/sample_project_tasks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sahaf\Desktop\Mohamed\Sahafintech\ekstrabooks-v2.0\public\uploads\media\default\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468E6D5F-1C53-4DDE-A29B-978C9F8CD505}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D14230E-C040-4E23-BFD4-1C77EDF097A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tasks" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>task code</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>PIPELINE WORKS</t>
+  </si>
+  <si>
+    <t>start_date</t>
+  </si>
+  <si>
+    <t>end_date</t>
   </si>
 </sst>
 </file>
@@ -98,9 +104,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,49 +413,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="15.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2">
+        <v>45048</v>
+      </c>
+      <c r="D2" s="2">
+        <v>45876</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>